<commit_message>
add citation message at end of program and in excell sheet
</commit_message>
<xml_diff>
--- a/excel_sheets/Degenerate-EC-VCD_For_Distribution.xlsx
+++ b/excel_sheets/Degenerate-EC-VCD_For_Distribution.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3120" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t xml:space="preserve">C </t>
   </si>
@@ -164,12 +164,46 @@
   <si>
     <t>R+(symmetric combination)</t>
   </si>
+  <si>
+    <r>
+      <t>Please cite “Determination of the Absolute Configurations Using Exciton Chirality Method for Vibrational Circular Dichroism: Right Answers for the Wrong Reasons?, C. L. Covington, V. P. Nicu, P.L.Polavarapu,  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>J. Phys. Chem. A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 2015, 119 (42), pp 10589–10601</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“ if you use these programs.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,8 +246,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +292,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -251,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -282,6 +342,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +665,7 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>44</v>
       </c>
@@ -612,7 +675,7 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -629,7 +692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -663,7 +726,7 @@
         <v>1.1483361999999999E-37</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>8</v>
       </c>
@@ -692,7 +755,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>9</v>
       </c>
@@ -722,7 +785,7 @@
         <v>1802.00665</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>2</v>
       </c>
@@ -742,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -762,12 +825,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -790,8 +853,18 @@
         <f>SQRT(C9^2+D9^2+E9^2)</f>
         <v>1.2065524970049999</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -815,12 +888,12 @@
         <v>1.2004600676111634</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F11" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -844,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -868,7 +941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -888,7 +961,7 @@
         <v>-1.1535105714285714</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1219,6 +1292,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H9:O9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>